<commit_message>
20120501-2 Nightly, Player Overview Box Scores & Split Stats done, fixed Box Scores btnOK
</commit_message>
<xml_diff>
--- a/teamorder.xlsx
+++ b/teamorder.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="45">
   <si>
     <t>Pistons</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>new 2</t>
+  </si>
+  <si>
+    <t>Mode 6</t>
   </si>
 </sst>
 </file>
@@ -496,21 +499,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -536,7 +540,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -544,7 +548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
@@ -555,7 +559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>22</v>
       </c>
@@ -566,7 +570,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -594,8 +598,11 @@
       <c r="I5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>28</v>
       </c>
@@ -609,7 +616,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11</v>
       </c>
@@ -622,8 +629,11 @@
       <c r="G7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12</v>
       </c>
@@ -636,8 +646,11 @@
       <c r="G8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -662,8 +675,11 @@
       <c r="I9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -688,8 +704,11 @@
       <c r="I10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>16</v>
       </c>
@@ -700,7 +719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -725,8 +744,11 @@
       <c r="I12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15</v>
       </c>
@@ -737,7 +759,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>27</v>
       </c>
@@ -751,7 +773,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -764,8 +786,11 @@
       <c r="G15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -790,8 +815,11 @@
       <c r="I16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>25</v>
       </c>
@@ -805,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>23</v>
       </c>
@@ -816,7 +844,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>29</v>
       </c>
@@ -830,7 +858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -841,7 +869,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -852,7 +880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -880,8 +908,11 @@
       <c r="I22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -909,8 +940,11 @@
       <c r="I23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -919,7 +953,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>26</v>
       </c>
@@ -933,7 +967,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>10</v>
       </c>
@@ -961,8 +995,11 @@
       <c r="I26" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>14</v>
       </c>
@@ -972,8 +1009,11 @@
       <c r="G27" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
@@ -987,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>17</v>
       </c>
@@ -998,7 +1038,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1009,7 +1049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>8</v>
       </c>
@@ -1034,8 +1074,11 @@
       <c r="I31" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>19</v>
       </c>
@@ -1046,7 +1089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33">
         <f>COUNTA(B3:B32)</f>
         <v>30</v>
@@ -1067,8 +1110,12 @@
         <f>COUNTA(F3:F32)</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <f t="shared" ref="J33" si="1">COUNTA(J2:J32)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>38</v>
       </c>
@@ -1086,6 +1133,9 @@
       </c>
       <c r="G34" t="s">
         <v>39</v>
+      </c>
+      <c r="J34" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>